<commit_message>
Update to remove conflicts from institute list -- and fix second appearance of Hampton
</commit_message>
<xml_diff>
--- a/11-CollaborationList/2022-05-23-LhARA-list.xlsx
+++ b/11-CollaborationList/2022-05-23-LhARA-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/CubMac-Home/CCAP/18-LhARA/00-Admin/00b-Collaboration-lists/11-CollaborationList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/00-Collaboration-lists/11-CollaborationList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A5014A-2FCE-B147-8BBA-98D20ABFC0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC302F3E-A629-2F49-89FE-0C65B8F1281F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2022-05-23-LhARA-list" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="554">
   <si>
     <t>Title</t>
   </si>
@@ -470,9 +470,6 @@
   </si>
   <si>
     <t>Department of Medical Physics, Hampton University Proton Therapy Institute, Hampton, VA 23666</t>
-  </si>
-  <si>
-    <t>Hampton University</t>
   </si>
   <si>
     <t>0000-0002-1378-3337</t>
@@ -2843,10 +2840,10 @@
   <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A50" sqref="A50:XFD50"/>
+      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3154,7 +3151,7 @@
         <v>77</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>78</v>
@@ -3436,11 +3433,9 @@
       <c r="I17" s="1">
         <v>1</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="8"/>
+      <c r="N17" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3448,25 +3443,25 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>125</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
@@ -3477,19 +3472,19 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>104</v>
@@ -3506,25 +3501,25 @@
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
@@ -3535,25 +3530,25 @@
         <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -3564,25 +3559,25 @@
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>125</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="I22" s="1">
         <v>1</v>
@@ -3599,34 +3594,34 @@
         <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="I23" s="1">
         <v>1</v>
       </c>
       <c r="J23" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3634,34 +3629,34 @@
         <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="I24" s="1">
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3669,31 +3664,31 @@
         <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E25" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3701,34 +3696,34 @@
         <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="I26" s="1">
         <v>1</v>
       </c>
       <c r="J26" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3736,19 +3731,19 @@
         <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>119</v>
@@ -3763,10 +3758,10 @@
         <v>121</v>
       </c>
       <c r="K27" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3774,31 +3769,31 @@
         <v>63</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>95</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I28" s="1">
         <v>0</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3806,25 +3801,25 @@
         <v>15</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="I29" s="1">
         <v>0</v>
@@ -3835,25 +3830,25 @@
         <v>15</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="I30" s="1">
         <v>0</v>
@@ -3864,25 +3859,25 @@
         <v>33</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="I31" s="1">
         <v>0</v>
@@ -3893,31 +3888,31 @@
         <v>15</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="F32" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="I32" s="1">
         <v>0</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3925,25 +3920,25 @@
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="I33" s="1">
         <v>0</v>
@@ -3954,31 +3949,31 @@
         <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="I34" s="1">
         <v>0</v>
       </c>
       <c r="O34" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3986,31 +3981,31 @@
         <v>63</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="F35" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O35" s="4"/>
     </row>
@@ -4019,25 +4014,25 @@
         <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="I36" s="1">
         <v>0</v>
@@ -4048,25 +4043,25 @@
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="G37" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="I37" s="1">
         <v>0</v>
@@ -4074,40 +4069,40 @@
     </row>
     <row r="38" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="G38" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="I38" s="1">
         <v>1</v>
       </c>
       <c r="J38" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="K38" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>254</v>
-      </c>
       <c r="N38" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4115,37 +4110,37 @@
         <v>15</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="I39" s="1">
         <v>1</v>
       </c>
       <c r="J39" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K39" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4153,34 +4148,34 @@
         <v>15</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>292</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G40" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="I40" s="1">
         <v>1</v>
       </c>
       <c r="J40" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="K40" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4188,25 +4183,25 @@
         <v>33</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>298</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="I41" s="1">
         <v>0</v>
@@ -4217,19 +4212,19 @@
         <v>15</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>306</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>21</v>
@@ -4246,25 +4241,25 @@
         <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="I43" s="1">
         <v>0</v>
@@ -4275,25 +4270,25 @@
         <v>33</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>314</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>316</v>
-      </c>
       <c r="G44" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I44" s="1">
         <v>1</v>
@@ -4302,7 +4297,7 @@
         <v>30</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4310,25 +4305,25 @@
         <v>33</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I45" s="1">
         <v>0</v>
@@ -4339,25 +4334,25 @@
         <v>33</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>328</v>
-      </c>
       <c r="G46" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="I46" s="1">
         <v>0</v>
@@ -4368,43 +4363,43 @@
         <v>15</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>333</v>
-      </c>
       <c r="G47" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I47" s="1">
         <v>2</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L47" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="M47" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="N47" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="N47" s="1" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4412,25 +4407,25 @@
         <v>15</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>342</v>
       </c>
       <c r="I48" s="1">
         <v>0</v>
@@ -4441,31 +4436,31 @@
         <v>72</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>346</v>
-      </c>
       <c r="G49" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="I49" s="1">
         <v>0</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="50" spans="1:15" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4473,37 +4468,37 @@
         <v>24</v>
       </c>
       <c r="B50" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="C50" s="17" t="s">
         <v>348</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>349</v>
       </c>
       <c r="D50" s="17" t="s">
         <v>92</v>
       </c>
       <c r="E50" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="F50" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="F50" s="17" t="s">
+      <c r="G50" s="17" t="s">
+        <v>552</v>
+      </c>
+      <c r="H50" s="17" t="s">
         <v>351</v>
-      </c>
-      <c r="G50" s="17" t="s">
-        <v>553</v>
-      </c>
-      <c r="H50" s="17" t="s">
-        <v>352</v>
       </c>
       <c r="I50" s="17">
         <v>1</v>
       </c>
       <c r="J50" s="17" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="K50" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="N50" s="19" t="s">
         <v>353</v>
-      </c>
-      <c r="N50" s="19" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4511,34 +4506,34 @@
         <v>24</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>356</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="I51" s="1">
         <v>1</v>
       </c>
       <c r="J51" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="K51" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4546,25 +4541,25 @@
         <v>33</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>362</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>365</v>
       </c>
       <c r="I52" s="1">
         <v>0</v>
@@ -4577,31 +4572,31 @@
         <v>72</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>367</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>125</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I53" s="1">
         <v>1</v>
       </c>
       <c r="J53" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K53" s="1" t="s">
         <v>334</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>335</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>41</v>
@@ -4612,34 +4607,34 @@
         <v>72</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>373</v>
-      </c>
       <c r="G54" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I54" s="1">
         <v>1</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4650,31 +4645,31 @@
         <v>50</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>95</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I55" s="1">
         <v>1</v>
       </c>
       <c r="J55" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="K55" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4682,34 +4677,34 @@
         <v>33</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>382</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>384</v>
-      </c>
       <c r="G56" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="I56" s="1">
         <v>1</v>
       </c>
       <c r="J56" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K56" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4717,25 +4712,25 @@
         <v>15</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="I57" s="1">
         <v>0</v>
@@ -4746,25 +4741,25 @@
         <v>33</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>125</v>
       </c>
       <c r="E58" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="G58" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>395</v>
       </c>
       <c r="I58" s="1">
         <v>0</v>
@@ -4775,37 +4770,37 @@
         <v>15</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>400</v>
-      </c>
       <c r="G59" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I59" s="1">
         <v>1</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4813,19 +4808,19 @@
         <v>15</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>406</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>47</v>
@@ -4837,7 +4832,7 @@
         <v>0</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4845,31 +4840,31 @@
         <v>24</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="E61" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="F61" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>411</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>111</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I61" s="1">
         <v>0</v>
       </c>
       <c r="N61" s="13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4877,19 +4872,19 @@
         <v>33</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="F62" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>104</v>
@@ -4906,19 +4901,19 @@
         <v>33</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E63" s="1" t="s">
+      <c r="F63" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>128</v>
@@ -4930,7 +4925,7 @@
         <v>0</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4938,34 +4933,34 @@
         <v>15</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="E64" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="F64" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="G64" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="H64" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="I64" s="1">
         <v>1</v>
       </c>
       <c r="J64" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="K64" s="1" t="s">
         <v>431</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4973,25 +4968,25 @@
         <v>33</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>434</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>436</v>
-      </c>
       <c r="G65" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I65" s="1">
         <v>1</v>
@@ -5008,25 +5003,25 @@
         <v>15</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="E66" s="1" t="s">
+      <c r="F66" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="G66" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="G66" s="1" t="s">
+      <c r="H66" s="1" t="s">
         <v>441</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>442</v>
       </c>
       <c r="I66" s="1">
         <v>0</v>
@@ -5037,34 +5032,34 @@
         <v>33</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>444</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E67" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>446</v>
-      </c>
       <c r="G67" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I67" s="1">
         <v>2</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>30</v>
@@ -5078,37 +5073,37 @@
         <v>33</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="E68" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="F68" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>451</v>
-      </c>
       <c r="G68" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="H68" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="I68" s="1">
         <v>1</v>
       </c>
       <c r="J68" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="K68" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="K68" s="1" t="s">
+      <c r="N68" s="1" t="s">
         <v>453</v>
-      </c>
-      <c r="N68" s="1" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5116,25 +5111,25 @@
         <v>15</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>456</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E69" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>458</v>
-      </c>
       <c r="G69" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="H69" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="I69" s="1">
         <v>0</v>
@@ -5145,19 +5140,19 @@
         <v>33</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E70" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>460</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>461</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>21</v>
@@ -5174,31 +5169,31 @@
         <v>15</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="E71" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="F71" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="G71" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="G71" s="1" t="s">
+      <c r="H71" s="1" t="s">
         <v>467</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>468</v>
       </c>
       <c r="I71" s="1">
         <v>0</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5206,19 +5201,19 @@
         <v>33</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="E72" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="F72" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>474</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>97</v>
@@ -5235,19 +5230,19 @@
         <v>15</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>476</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E73" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>477</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>478</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>111</v>
@@ -5273,22 +5268,22 @@
         <v>34</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E74" s="1" t="s">
+      <c r="F74" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>481</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I74" s="1">
         <v>0</v>
@@ -5299,25 +5294,25 @@
         <v>33</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="E75" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="F75" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="F75" s="1" t="s">
+      <c r="G75" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="G75" s="1" t="s">
+      <c r="H75" s="1" t="s">
         <v>487</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>488</v>
       </c>
       <c r="I75" s="1">
         <v>0</v>
@@ -5328,34 +5323,34 @@
         <v>15</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="E76" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="F76" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="G76" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="G76" s="1" t="s">
+      <c r="H76" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>495</v>
       </c>
       <c r="I76" s="1">
         <v>1</v>
       </c>
       <c r="J76" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="K76" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5366,16 +5361,16 @@
         <v>80</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E77" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="F77" s="1" t="s">
         <v>499</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>500</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>119</v>
@@ -5392,25 +5387,25 @@
         <v>15</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="E78" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="F78" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>505</v>
-      </c>
       <c r="G78" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5418,34 +5413,34 @@
         <v>33</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="D79" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E79" s="1" t="s">
+      <c r="F79" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>509</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>95</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I79" s="1">
         <v>1</v>
       </c>
       <c r="J79" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="K79" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="K79" s="1" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5453,31 +5448,31 @@
         <v>72</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>510</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>511</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E80" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>513</v>
-      </c>
       <c r="G80" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I80" s="1">
         <v>0</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5485,19 +5480,19 @@
         <v>33</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E81" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>516</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>517</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>30</v>
@@ -5514,25 +5509,25 @@
         <v>24</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E82" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="G82" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="G82" s="1" t="s">
+      <c r="H82" s="1" t="s">
         <v>521</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>522</v>
       </c>
       <c r="I82" s="1">
         <v>0</v>
@@ -5543,25 +5538,25 @@
         <v>15</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E83" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>525</v>
-      </c>
       <c r="G83" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H83" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="I83" s="1">
         <v>0</v>
@@ -5572,25 +5567,25 @@
         <v>15</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="E84" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="F84" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>530</v>
-      </c>
       <c r="G84" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H84" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="I84" s="1">
         <v>1</v>
@@ -5602,7 +5597,7 @@
         <v>88</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5610,19 +5605,19 @@
         <v>33</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="D85" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D85" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E85" s="1" t="s">
+      <c r="F85" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>535</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>21</v>
@@ -5639,34 +5634,34 @@
         <v>33</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E86" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E86" s="1" t="s">
+      <c r="F86" s="1" t="s">
         <v>538</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>539</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>95</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I86" s="1">
         <v>1</v>
       </c>
       <c r="J86" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="K86" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="K86" s="1" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5674,25 +5669,25 @@
         <v>72</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>541</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E87" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="F87" s="1" t="s">
+      <c r="G87" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="G87" s="1" t="s">
+      <c r="H87" s="1" t="s">
         <v>544</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>545</v>
       </c>
       <c r="I87" s="1">
         <v>0</v>
@@ -5703,25 +5698,25 @@
         <v>72</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E88" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>550</v>
-      </c>
       <c r="G88" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H88" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="I88" s="1">
         <v>0</v>
@@ -5747,6 +5742,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085CA6C7F4A4AB74096FC0EC2FFBCDC1B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ae49459f8d36ac24e5b40f725d622ad4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d2c9d8e6-4447-41a5-9589-9fed66499f9c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ac636e76d545aa2779bc08ab2e67d1b" ns2:_="">
     <xsd:import namespace="d2c9d8e6-4447-41a5-9589-9fed66499f9c"/>
@@ -5892,35 +5902,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDA5C47C-E79B-4ED5-99E2-D9DF528E7178}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D201AF0C-D84D-4646-898F-B45F73A20A95}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d2c9d8e6-4447-41a5-9589-9fed66499f9c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5942,9 +5927,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D201AF0C-D84D-4646-898F-B45F73A20A95}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDA5C47C-E79B-4ED5-99E2-D9DF528E7178}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d2c9d8e6-4447-41a5-9589-9fed66499f9c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>